<commit_message>
exel generate css code
</commit_message>
<xml_diff>
--- a/ChlildN.xlsx
+++ b/ChlildN.xlsx
@@ -21,6 +21,10 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -371,20 +375,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C1:H14"/>
+  <dimension ref="C1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="I3" sqref="I3:I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="9" max="9" width="88.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C1">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C2">
         <v>60</v>
       </c>
@@ -396,7 +403,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C3">
         <v>0</v>
       </c>
@@ -419,8 +426,16 @@
       <c r="H3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="I3" t="str">
+        <f>".filter-btn.open .panelTool:nth-child("&amp;H3&amp;") {   transform: translate("&amp;INT(G3)&amp;"px, "&amp;INT(F3)&amp;"px); }"</f>
+        <v>.filter-btn.open .panelTool:nth-child(1) {   transform: translate(31px, -55px); }</v>
+      </c>
+      <c r="J3" t="str">
+        <f>""</f>
+        <v/>
+      </c>
+    </row>
+    <row r="4" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C4">
         <v>1</v>
       </c>
@@ -443,8 +458,12 @@
       <c r="H4">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="I4" t="str">
+        <f t="shared" ref="I4:I14" si="4">".filter-btn.open .panelTool:nth-child("&amp;H4&amp;") {   transform: translate("&amp;INT(G4)&amp;"px, "&amp;INT(F4)&amp;"px); }"</f>
+        <v>.filter-btn.open .panelTool:nth-child(2) {   transform: translate(8px, -63px); }</v>
+      </c>
+    </row>
+    <row r="5" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C5">
         <v>2</v>
       </c>
@@ -467,8 +486,12 @@
       <c r="H5">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="I5" t="str">
+        <f t="shared" si="4"/>
+        <v>.filter-btn.open .panelTool:nth-child(3) {   transform: translate(-15px, -62px); }</v>
+      </c>
+    </row>
+    <row r="6" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C6">
         <v>3</v>
       </c>
@@ -491,8 +514,12 @@
       <c r="H6">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="I6" t="str">
+        <f t="shared" si="4"/>
+        <v>.filter-btn.open .panelTool:nth-child(4) {   transform: translate(-37px, -52px); }</v>
+      </c>
+    </row>
+    <row r="7" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C7">
         <v>4</v>
       </c>
@@ -515,8 +542,12 @@
       <c r="H7">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="I7" t="str">
+        <f t="shared" si="4"/>
+        <v>.filter-btn.open .panelTool:nth-child(5) {   transform: translate(-53px, -35px); }</v>
+      </c>
+    </row>
+    <row r="8" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C8">
         <v>5</v>
       </c>
@@ -539,8 +570,12 @@
       <c r="H8">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="I8" t="str">
+        <f t="shared" si="4"/>
+        <v>.filter-btn.open .panelTool:nth-child(6) {   transform: translate(-62px, -12px); }</v>
+      </c>
+    </row>
+    <row r="9" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C9">
         <v>6</v>
       </c>
@@ -563,8 +598,12 @@
       <c r="H9">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="I9" t="str">
+        <f t="shared" si="4"/>
+        <v>.filter-btn.open .panelTool:nth-child(7) {   transform: translate(-62px, 11px); }</v>
+      </c>
+    </row>
+    <row r="10" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C10">
         <v>7</v>
       </c>
@@ -587,8 +626,12 @@
       <c r="H10">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="I10" t="str">
+        <f t="shared" si="4"/>
+        <v>.filter-btn.open .panelTool:nth-child(8) {   transform: translate(-53px, 34px); }</v>
+      </c>
+    </row>
+    <row r="11" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C11">
         <v>8</v>
       </c>
@@ -611,8 +654,12 @@
       <c r="H11">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="I11" t="str">
+        <f t="shared" si="4"/>
+        <v>.filter-btn.open .panelTool:nth-child(9) {   transform: translate(-37px, 51px); }</v>
+      </c>
+    </row>
+    <row r="12" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C12">
         <v>9</v>
       </c>
@@ -635,8 +682,12 @@
       <c r="H12">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="I12" t="str">
+        <f t="shared" si="4"/>
+        <v>.filter-btn.open .panelTool:nth-child(10) {   transform: translate(-15px, 61px); }</v>
+      </c>
+    </row>
+    <row r="13" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C13">
         <v>10</v>
       </c>
@@ -659,8 +710,12 @@
       <c r="H13">
         <v>11</v>
       </c>
-    </row>
-    <row r="14" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="I13" t="str">
+        <f t="shared" si="4"/>
+        <v>.filter-btn.open .panelTool:nth-child(11) {   transform: translate(8px, 62px); }</v>
+      </c>
+    </row>
+    <row r="14" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C14">
         <v>11</v>
       </c>
@@ -682,6 +737,10 @@
       </c>
       <c r="H14">
         <v>12</v>
+      </c>
+      <c r="I14" t="str">
+        <f t="shared" si="4"/>
+        <v>.filter-btn.open .panelTool:nth-child(12) {   transform: translate(31px, 54px); }</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
correct css static generated
</commit_message>
<xml_diff>
--- a/ChlildN.xlsx
+++ b/ChlildN.xlsx
@@ -378,7 +378,7 @@
   <dimension ref="C1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3:I13"/>
+      <selection activeCell="I3" sqref="I3:I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -388,7 +388,7 @@
   <sheetData>
     <row r="1" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C1">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="3:10" x14ac:dyDescent="0.3">
@@ -397,7 +397,7 @@
       </c>
       <c r="D2">
         <f>(360-2*$C$2)/$C$1</f>
-        <v>21.818181818181817</v>
+        <v>24</v>
       </c>
       <c r="F2">
         <v>63</v>
@@ -441,26 +441,26 @@
       </c>
       <c r="D4">
         <f t="shared" ref="D4:D14" si="0">$C$2+C4*$D$2</f>
-        <v>81.818181818181813</v>
+        <v>84</v>
       </c>
       <c r="E4">
         <f t="shared" ref="E4:E14" si="1">D4*PI()/180</f>
-        <v>1.4279966607226331</v>
+        <v>1.4660765716752369</v>
       </c>
       <c r="F4" s="1">
         <f t="shared" ref="F4:F14" si="2">-SIN($E4)*$F$2</f>
-        <v>-62.358750838498757</v>
+        <v>-62.654879408201218</v>
       </c>
       <c r="G4" s="1">
         <f t="shared" ref="G4:G14" si="3">COS($E4)*$F$2</f>
-        <v>8.9658348112169755</v>
+        <v>6.5852931858621675</v>
       </c>
       <c r="H4">
         <v>2</v>
       </c>
       <c r="I4" t="str">
         <f t="shared" ref="I4:I14" si="4">".filter-btn.open .panelTool:nth-child("&amp;H4&amp;") {   transform: translate("&amp;INT(G4)&amp;"px, "&amp;INT(F4)&amp;"px); }"</f>
-        <v>.filter-btn.open .panelTool:nth-child(2) {   transform: translate(8px, -63px); }</v>
+        <v>.filter-btn.open .panelTool:nth-child(2) {   transform: translate(6px, -63px); }</v>
       </c>
     </row>
     <row r="5" spans="3:10" x14ac:dyDescent="0.3">
@@ -469,26 +469,26 @@
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
-        <v>103.63636363636363</v>
+        <v>108</v>
       </c>
       <c r="E5">
         <f t="shared" si="1"/>
-        <v>1.8087957702486686</v>
+        <v>1.8849555921538759</v>
       </c>
       <c r="F5" s="1">
         <f t="shared" si="2"/>
-        <v>-61.224128804383128</v>
+        <v>-59.916560526594679</v>
       </c>
       <c r="G5" s="1">
         <f t="shared" si="3"/>
-        <v>-14.852812937093898</v>
+        <v>-19.468070645621683</v>
       </c>
       <c r="H5">
         <v>3</v>
       </c>
       <c r="I5" t="str">
         <f t="shared" si="4"/>
-        <v>.filter-btn.open .panelTool:nth-child(3) {   transform: translate(-15px, -62px); }</v>
+        <v>.filter-btn.open .panelTool:nth-child(3) {   transform: translate(-20px, -60px); }</v>
       </c>
     </row>
     <row r="6" spans="3:10" x14ac:dyDescent="0.3">
@@ -497,26 +497,26 @@
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
-        <v>125.45454545454545</v>
+        <v>132</v>
       </c>
       <c r="E6">
         <f t="shared" si="1"/>
-        <v>2.1895948797747042</v>
+        <v>2.3038346126325151</v>
       </c>
       <c r="F6" s="1">
         <f t="shared" si="2"/>
-        <v>-51.31828497917116</v>
+        <v>-46.818124005075838</v>
       </c>
       <c r="G6" s="1">
         <f>COS($E6)*$F$2</f>
-        <v>-36.543585302985477</v>
+        <v>-42.155228200608072</v>
       </c>
       <c r="H6">
         <v>4</v>
       </c>
       <c r="I6" t="str">
         <f t="shared" si="4"/>
-        <v>.filter-btn.open .panelTool:nth-child(4) {   transform: translate(-37px, -52px); }</v>
+        <v>.filter-btn.open .panelTool:nth-child(4) {   transform: translate(-43px, -47px); }</v>
       </c>
     </row>
     <row r="7" spans="3:10" x14ac:dyDescent="0.3">
@@ -525,26 +525,26 @@
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
-        <v>147.27272727272725</v>
+        <v>156</v>
       </c>
       <c r="E7">
         <f t="shared" si="1"/>
-        <v>2.5703939893007397</v>
+        <v>2.7227136331111539</v>
       </c>
       <c r="F7" s="1">
         <f t="shared" si="2"/>
-        <v>-34.060371499702661</v>
+        <v>-25.624408513775428</v>
       </c>
       <c r="G7" s="1">
         <f t="shared" si="3"/>
-        <v>-52.998972568364408</v>
+        <v>-57.55336383148385</v>
       </c>
       <c r="H7">
         <v>5</v>
       </c>
       <c r="I7" t="str">
         <f t="shared" si="4"/>
-        <v>.filter-btn.open .panelTool:nth-child(5) {   transform: translate(-53px, -35px); }</v>
+        <v>.filter-btn.open .panelTool:nth-child(5) {   transform: translate(-58px, -26px); }</v>
       </c>
     </row>
     <row r="8" spans="3:10" x14ac:dyDescent="0.3">
@@ -553,26 +553,26 @@
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
-        <v>169.09090909090907</v>
+        <v>180</v>
       </c>
       <c r="E8">
         <f t="shared" si="1"/>
-        <v>2.9511930988267752</v>
+        <v>3.1415926535897931</v>
       </c>
       <c r="F8" s="1">
         <f t="shared" si="2"/>
-        <v>-11.922828394705862</v>
+        <v>-7.7184352659243061E-15</v>
       </c>
       <c r="G8" s="1">
         <f t="shared" si="3"/>
-        <v>-61.861507927550512</v>
+        <v>-63</v>
       </c>
       <c r="H8">
         <v>6</v>
       </c>
       <c r="I8" t="str">
         <f t="shared" si="4"/>
-        <v>.filter-btn.open .panelTool:nth-child(6) {   transform: translate(-62px, -12px); }</v>
+        <v>.filter-btn.open .panelTool:nth-child(6) {   transform: translate(-63px, -1px); }</v>
       </c>
     </row>
     <row r="9" spans="3:10" x14ac:dyDescent="0.3">
@@ -581,26 +581,26 @@
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
-        <v>190.90909090909091</v>
+        <v>204</v>
       </c>
       <c r="E9">
         <f t="shared" si="1"/>
-        <v>3.3319922083528106</v>
+        <v>3.5604716740684319</v>
       </c>
       <c r="F9" s="1">
         <f t="shared" si="2"/>
-        <v>11.922828394705819</v>
+        <v>25.624408513775389</v>
       </c>
       <c r="G9" s="1">
         <f t="shared" si="3"/>
-        <v>-61.861507927550527</v>
+        <v>-57.553363831483871</v>
       </c>
       <c r="H9">
         <v>7</v>
       </c>
       <c r="I9" t="str">
         <f t="shared" si="4"/>
-        <v>.filter-btn.open .panelTool:nth-child(7) {   transform: translate(-62px, 11px); }</v>
+        <v>.filter-btn.open .panelTool:nth-child(7) {   transform: translate(-58px, 25px); }</v>
       </c>
     </row>
     <row r="10" spans="3:10" x14ac:dyDescent="0.3">
@@ -609,26 +609,26 @@
       </c>
       <c r="D10">
         <f t="shared" si="0"/>
-        <v>212.72727272727272</v>
+        <v>228</v>
       </c>
       <c r="E10">
         <f t="shared" si="1"/>
-        <v>3.7127913178788465</v>
+        <v>3.9793506945470711</v>
       </c>
       <c r="F10" s="1">
         <f t="shared" si="2"/>
-        <v>34.060371499702647</v>
+        <v>46.818124005075823</v>
       </c>
       <c r="G10" s="1">
         <f t="shared" si="3"/>
-        <v>-52.998972568364415</v>
+        <v>-42.155228200608086</v>
       </c>
       <c r="H10">
         <v>8</v>
       </c>
       <c r="I10" t="str">
         <f t="shared" si="4"/>
-        <v>.filter-btn.open .panelTool:nth-child(8) {   transform: translate(-53px, 34px); }</v>
+        <v>.filter-btn.open .panelTool:nth-child(8) {   transform: translate(-43px, 46px); }</v>
       </c>
     </row>
     <row r="11" spans="3:10" x14ac:dyDescent="0.3">
@@ -637,26 +637,26 @@
       </c>
       <c r="D11">
         <f t="shared" si="0"/>
-        <v>234.54545454545453</v>
+        <v>252</v>
       </c>
       <c r="E11">
         <f t="shared" si="1"/>
-        <v>4.093590427404882</v>
+        <v>4.3982297150257104</v>
       </c>
       <c r="F11" s="1">
         <f t="shared" si="2"/>
-        <v>51.318284979171146</v>
+        <v>59.916560526594672</v>
       </c>
       <c r="G11" s="1">
         <f t="shared" si="3"/>
-        <v>-36.543585302985491</v>
+        <v>-19.468070645621697</v>
       </c>
       <c r="H11">
         <v>9</v>
       </c>
       <c r="I11" t="str">
         <f t="shared" si="4"/>
-        <v>.filter-btn.open .panelTool:nth-child(9) {   transform: translate(-37px, 51px); }</v>
+        <v>.filter-btn.open .panelTool:nth-child(9) {   transform: translate(-20px, 59px); }</v>
       </c>
     </row>
     <row r="12" spans="3:10" x14ac:dyDescent="0.3">
@@ -665,26 +665,26 @@
       </c>
       <c r="D12">
         <f t="shared" si="0"/>
-        <v>256.36363636363637</v>
+        <v>276</v>
       </c>
       <c r="E12">
         <f t="shared" si="1"/>
-        <v>4.4743895369309179</v>
+        <v>4.8171087355043491</v>
       </c>
       <c r="F12" s="1">
         <f t="shared" si="2"/>
-        <v>61.224128804383128</v>
+        <v>62.654879408201225</v>
       </c>
       <c r="G12" s="1">
         <f t="shared" si="3"/>
-        <v>-14.852812937093899</v>
+        <v>6.5852931858621382</v>
       </c>
       <c r="H12">
         <v>10</v>
       </c>
       <c r="I12" t="str">
         <f t="shared" si="4"/>
-        <v>.filter-btn.open .panelTool:nth-child(10) {   transform: translate(-15px, 61px); }</v>
+        <v>.filter-btn.open .panelTool:nth-child(10) {   transform: translate(6px, 62px); }</v>
       </c>
     </row>
     <row r="13" spans="3:10" x14ac:dyDescent="0.3">
@@ -693,26 +693,26 @@
       </c>
       <c r="D13">
         <f t="shared" si="0"/>
-        <v>278.18181818181813</v>
+        <v>300</v>
       </c>
       <c r="E13">
         <f t="shared" si="1"/>
-        <v>4.855188646456952</v>
+        <v>5.2359877559829888</v>
       </c>
       <c r="F13" s="1">
         <f t="shared" si="2"/>
-        <v>62.358750838498771</v>
+        <v>54.559600438419629</v>
       </c>
       <c r="G13" s="1">
         <f t="shared" si="3"/>
-        <v>8.965834811216892</v>
+        <v>31.500000000000007</v>
       </c>
       <c r="H13">
         <v>11</v>
       </c>
       <c r="I13" t="str">
         <f t="shared" si="4"/>
-        <v>.filter-btn.open .panelTool:nth-child(11) {   transform: translate(8px, 62px); }</v>
+        <v>.filter-btn.open .panelTool:nth-child(11) {   transform: translate(31px, 54px); }</v>
       </c>
     </row>
     <row r="14" spans="3:10" x14ac:dyDescent="0.3">
@@ -721,26 +721,26 @@
       </c>
       <c r="D14">
         <f t="shared" si="0"/>
-        <v>300</v>
+        <v>324</v>
       </c>
       <c r="E14">
         <f t="shared" si="1"/>
-        <v>5.2359877559829888</v>
+        <v>5.6548667764616276</v>
       </c>
       <c r="F14" s="1">
         <f t="shared" si="2"/>
-        <v>54.559600438419629</v>
+        <v>37.030470894425818</v>
       </c>
       <c r="G14" s="1">
         <f t="shared" si="3"/>
-        <v>31.500000000000007</v>
+        <v>50.96807064562168</v>
       </c>
       <c r="H14">
         <v>12</v>
       </c>
       <c r="I14" t="str">
         <f t="shared" si="4"/>
-        <v>.filter-btn.open .panelTool:nth-child(12) {   transform: translate(31px, 54px); }</v>
+        <v>.filter-btn.open .panelTool:nth-child(12) {   transform: translate(50px, 37px); }</v>
       </c>
     </row>
   </sheetData>

</xml_diff>